<commit_message>
se agrega imagen actualizada de la arquitectura
</commit_message>
<xml_diff>
--- a/documentos/V2_DATOS DE ALUMNO-DOCENTES-APORDEADO-DIRECTOR -VERSION ACTUALIZADO.xlsx
+++ b/documentos/V2_DATOS DE ALUMNO-DOCENTES-APORDEADO-DIRECTOR -VERSION ACTUALIZADO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AADD44F-8228-4B0B-B279-1E30C8CC002E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C121BC-4EFC-41C6-A0AA-9539F866C01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTADO DE PROFESOR X CURSO" sheetId="1" r:id="rId1"/>
@@ -9227,9 +9227,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9241,6 +9238,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9580,14 +9580,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="5" t="s">
         <v>2629</v>
       </c>
@@ -10084,14 +10084,14 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="41"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -10544,12 +10544,12 @@
     <mergeCell ref="B21:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:C16">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>$B$23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>$E$23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10560,11 +10560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAE5A96-FF54-427F-93BA-185A7F051C9F}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A2:N198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10576,15 +10575,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="41" t="s">
         <v>2677</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
@@ -10663,7 +10662,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00001','CM045','DO-27845671','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>2685</v>
@@ -10706,7 +10705,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00002','CM045','DO-27845671','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2686</v>
       </c>
@@ -10790,7 +10789,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00004','CM045','DO-27845671','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>2688</v>
@@ -10833,7 +10832,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00005','CM045','DO-27845671','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>2689</v>
@@ -10919,7 +10918,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00007','CM045','DO-27845671','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>2691</v>
@@ -10962,7 +10961,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00008','CM045','DO-27845671','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>2692</v>
@@ -11047,7 +11046,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00010','CM046','DO-21851329','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2695</v>
       </c>
@@ -11089,7 +11088,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00011','CM046','DO-21851329','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>2696</v>
@@ -11175,7 +11174,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00013','CM046','DO-21851329','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>2698</v>
@@ -11218,7 +11217,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00014','CM046','DO-21851329','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>2699</v>
@@ -11304,7 +11303,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00016','CM046','DO-21851329','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>2701</v>
@@ -11347,7 +11346,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00017','CM046','DO-21851329','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2702</v>
       </c>
@@ -11431,7 +11430,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00019','CM046','DO-21851329','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2704</v>
       </c>
@@ -11473,7 +11472,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00020','CM046','DO-21851329','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2705</v>
       </c>
@@ -11557,7 +11556,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00022','CM046','DO-21851329','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>2707</v>
       </c>
@@ -11599,7 +11598,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00023','CM046','DO-21851329','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2708</v>
       </c>
@@ -11683,7 +11682,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00025','CM047','DO-09755072','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2711</v>
       </c>
@@ -11725,7 +11724,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00026','CM047','DO-09755072','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>2712</v>
       </c>
@@ -11809,7 +11808,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00028','CM047','DO-09755072','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2714</v>
       </c>
@@ -11851,7 +11850,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00029','CM047','DO-09755072','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="33" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>2715</v>
       </c>
@@ -11935,7 +11934,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00031','CM047','DO-09755072','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="35" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>2717</v>
       </c>
@@ -11977,7 +11976,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00032','CM047','DO-09755072','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="36" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>2718</v>
       </c>
@@ -12061,7 +12060,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00034','CM048','DO-40346626','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="38" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>2721</v>
       </c>
@@ -12103,7 +12102,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00035','CM048','DO-40346626','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="39" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>2722</v>
       </c>
@@ -12187,7 +12186,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00037','CM048','DO-40346626','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="41" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>2724</v>
       </c>
@@ -12229,7 +12228,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00038','CM048','DO-40346626','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="42" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>2725</v>
       </c>
@@ -12313,7 +12312,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00040','CM048','DO-40346626','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="44" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>2727</v>
       </c>
@@ -12355,7 +12354,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00041','CM048','DO-40346626','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="45" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>2728</v>
       </c>
@@ -12439,7 +12438,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00043','CM048','DO-40346626','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="47" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>2731</v>
       </c>
@@ -12481,7 +12480,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00044','CM048','DO-40346626','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="48" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>2732</v>
       </c>
@@ -12565,7 +12564,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00046','CM048','DO-40346626','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="50" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>2734</v>
       </c>
@@ -12607,7 +12606,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00047','CM048','DO-40346626','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="51" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>2735</v>
       </c>
@@ -12691,7 +12690,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00049','CM049','DO-22246581','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="53" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>2737</v>
       </c>
@@ -12733,7 +12732,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00050','CM049','DO-22246581','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="54" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>2738</v>
       </c>
@@ -12817,7 +12816,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00052','CM049','DO-22246581','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="56" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>2741</v>
       </c>
@@ -12859,7 +12858,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00053','CM049','DO-22246581','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="57" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>2742</v>
       </c>
@@ -12943,7 +12942,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00055','CM049','DO-22246581','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="59" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>2744</v>
       </c>
@@ -12985,7 +12984,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00056','CM049','DO-22246581','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="60" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>2745</v>
       </c>
@@ -13069,7 +13068,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00058','CM049','DO-22246581','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="62" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>2747</v>
       </c>
@@ -13111,7 +13110,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00059','CM049','DO-22246581','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="63" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>2748</v>
       </c>
@@ -13195,7 +13194,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00061','CM049','DO-22246581','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="65" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>2751</v>
       </c>
@@ -13237,7 +13236,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00062','CM049','DO-22246581','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="66" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>2752</v>
       </c>
@@ -13321,7 +13320,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00064','CM050','DO-34912340','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="68" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>2754</v>
       </c>
@@ -13363,7 +13362,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00065','CM050','DO-34912340','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="69" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>2755</v>
       </c>
@@ -13447,7 +13446,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00067','CM050','DO-34912340','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="71" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>2757</v>
       </c>
@@ -13489,7 +13488,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00068','CM050','DO-34912340','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="72" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>2758</v>
       </c>
@@ -13573,7 +13572,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00070','CM050','DO-34912340','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="74" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>2761</v>
       </c>
@@ -13615,7 +13614,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00071','CM050','DO-34912340','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="75" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>2762</v>
       </c>
@@ -13699,7 +13698,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00073','CM050','DO-34912340','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="77" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>2764</v>
       </c>
@@ -13741,7 +13740,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00074','CM050','DO-34912340','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="78" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>2765</v>
       </c>
@@ -13825,7 +13824,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00076','CM050','DO-34912340','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="80" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>2767</v>
       </c>
@@ -13867,7 +13866,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00077','CM050','DO-34912340','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="81" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>2768</v>
       </c>
@@ -13951,7 +13950,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00079','CM051','DO-09755072','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="83" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>2771</v>
       </c>
@@ -13993,7 +13992,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00080','CM051','DO-09755072','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="84" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>2772</v>
       </c>
@@ -14077,7 +14076,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00082','CM051','DO-09755072','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="86" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>2774</v>
       </c>
@@ -14119,7 +14118,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00083','CM051','DO-09755072','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="87" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>2775</v>
       </c>
@@ -14203,7 +14202,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00085','CM051','DO-09755072','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="89" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>2777</v>
       </c>
@@ -14245,7 +14244,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00086','CM051','DO-09755072','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="90" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>2778</v>
       </c>
@@ -14329,7 +14328,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00088','CM051','DO-09755072','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="92" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>2781</v>
       </c>
@@ -14371,7 +14370,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00089','CM051','DO-09755072','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="93" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>2782</v>
       </c>
@@ -14455,7 +14454,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00091','CM051','DO-09755072','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="95" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>2784</v>
       </c>
@@ -14497,7 +14496,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00092','CM051','DO-09755072','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="96" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>2785</v>
       </c>
@@ -14581,7 +14580,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00094','CM052','DO-56432890','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="98" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>2787</v>
       </c>
@@ -14623,7 +14622,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00095','CM052','DO-56432890','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="99" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>2788</v>
       </c>
@@ -14707,7 +14706,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00097','CM052','DO-56432890','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="101" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>2791</v>
       </c>
@@ -14749,7 +14748,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00098','CM052','DO-56432890','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="102" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>2792</v>
       </c>
@@ -14833,7 +14832,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00100','CM052','DO-56432890','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="104" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>2794</v>
       </c>
@@ -14875,7 +14874,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00101','CM052','DO-56432890','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="105" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>2795</v>
       </c>
@@ -14959,7 +14958,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00103','CM052','DO-56432890','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="107" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>2797</v>
       </c>
@@ -15001,7 +15000,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00104','CM052','DO-56432890','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="108" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>2798</v>
       </c>
@@ -15085,7 +15084,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00106','CM052','DO-56432890','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="110" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>2801</v>
       </c>
@@ -15127,7 +15126,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00107','CM052','DO-56432890','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="111" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>2802</v>
       </c>
@@ -15211,7 +15210,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00109','CM053','DO-80615241','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="113" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>2804</v>
       </c>
@@ -15253,7 +15252,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00110','CM053','DO-80615241','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="114" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>2805</v>
       </c>
@@ -15337,7 +15336,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00112','CM053','DO-80615241','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="116" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>2807</v>
       </c>
@@ -15379,7 +15378,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00113','CM053','DO-80615241','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="117" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>2808</v>
       </c>
@@ -15463,7 +15462,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00115','CM053','DO-80615241','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="119" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>2811</v>
       </c>
@@ -15505,7 +15504,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00116','CM053','DO-80615241','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="120" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>2812</v>
       </c>
@@ -15589,7 +15588,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00118','CM054','DO-72613922','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="122" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>2814</v>
       </c>
@@ -15631,7 +15630,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00119','CM054','DO-72613922','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="123" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>2815</v>
       </c>
@@ -15715,7 +15714,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00121','CM054','DO-72613922','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="125" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>2817</v>
       </c>
@@ -15757,7 +15756,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00122','CM054','DO-72613922','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="126" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>2818</v>
       </c>
@@ -15841,7 +15840,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00124','CM054','DO-72613922','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="128" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>2832</v>
       </c>
@@ -15883,7 +15882,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00125','CM054','DO-72613922','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="129" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>2833</v>
       </c>
@@ -15967,7 +15966,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00127','CM054','DO-72613922','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="131" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>2835</v>
       </c>
@@ -16009,7 +16008,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00128','CM054','DO-72613922','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="132" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>2836</v>
       </c>
@@ -16093,7 +16092,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00130','CM054','DO-72613922','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="134" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>2838</v>
       </c>
@@ -16135,7 +16134,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00131','CM054','DO-72613922','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="135" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>2839</v>
       </c>
@@ -16219,7 +16218,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00133','CM055','DO-21843146','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="137" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>2841</v>
       </c>
@@ -16261,7 +16260,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00134','CM055','DO-21843146','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="138" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>2842</v>
       </c>
@@ -16345,7 +16344,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00136','CM055','DO-21843146','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="140" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>2844</v>
       </c>
@@ -16387,7 +16386,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00137','CM055','DO-21843146','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="141" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>2845</v>
       </c>
@@ -16471,7 +16470,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00139','CM055','DO-21843146','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="143" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>2847</v>
       </c>
@@ -16513,7 +16512,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00140','CM055','DO-21843146','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="144" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>2848</v>
       </c>
@@ -16555,7 +16554,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00141','CM055','DO-21843146','ZOOM','C','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="145" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>2849</v>
       </c>
@@ -16597,7 +16596,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00142','CM055','DO-21843146','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="146" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>2850</v>
       </c>
@@ -16681,7 +16680,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00144','CM055','DO-21843146','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="148" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>2852</v>
       </c>
@@ -16723,7 +16722,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00145','CM055','DO-21843146','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="149" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>2853</v>
       </c>
@@ -16765,7 +16764,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00146','CM055','DO-21843146','ZOOM','C','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="150" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>2854</v>
       </c>
@@ -16849,7 +16848,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00148','CM056','DO-09468871','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="152" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>2856</v>
       </c>
@@ -16891,7 +16890,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00149','CM056','DO-09468871','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="153" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>2857</v>
       </c>
@@ -16975,7 +16974,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00151','CM056','DO-09468871','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="155" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>2859</v>
       </c>
@@ -17017,7 +17016,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00152','CM056','DO-09468871','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="156" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>2860</v>
       </c>
@@ -17101,7 +17100,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00154','CM056','DO-09468871','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="158" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>2863</v>
       </c>
@@ -17143,7 +17142,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00155','CM056','DO-09468871','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="159" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>2864</v>
       </c>
@@ -17227,7 +17226,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00157','CM056','DO-25673536','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="161" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>2866</v>
       </c>
@@ -17269,7 +17268,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00158','CM056','DO-25673536','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="162" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>2867</v>
       </c>
@@ -17353,7 +17352,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00160','CM056','DO-25673536','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="164" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>2870</v>
       </c>
@@ -17395,7 +17394,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00161','CM056','DO-25673536','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="165" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>2871</v>
       </c>
@@ -17479,7 +17478,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00163','CM057','DO-23781004','ZOOM','A','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="167" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>2873</v>
       </c>
@@ -17521,7 +17520,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00164','CM057','DO-23781004','ZOOM','B','1','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="168" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>2874</v>
       </c>
@@ -17605,7 +17604,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00166','CM057','DO-23781004','ZOOM','A','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="170" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>2877</v>
       </c>
@@ -17647,7 +17646,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00167','CM057','DO-23781004','ZOOM','B','2','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="171" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>2878</v>
       </c>
@@ -17731,7 +17730,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00169','CM057','DO-23781004','ZOOM','A','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="173" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>2880</v>
       </c>
@@ -17773,7 +17772,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00170','CM057','DO-23781004','ZOOM','B','3','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="174" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>2881</v>
       </c>
@@ -17857,7 +17856,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00172','CM057','DO-23781004','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="176" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>2883</v>
       </c>
@@ -17899,7 +17898,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00173','CM057','DO-23781004','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="177" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>2885</v>
       </c>
@@ -17983,7 +17982,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00175','CM057','DO-23781004','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="179" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>2887</v>
       </c>
@@ -18025,7 +18024,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00176','CM057','DO-23781004','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="180" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>2888</v>
       </c>
@@ -18109,7 +18108,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00178','CM045','DO-38916309','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="182" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>2890</v>
       </c>
@@ -18151,7 +18150,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00179','CM045','DO-38916309','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="183" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>2891</v>
       </c>
@@ -18235,7 +18234,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00181','CM045','DO-38916309','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="185" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>2893</v>
       </c>
@@ -18277,7 +18276,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00182','CM045','DO-38916309','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="186" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>2894</v>
       </c>
@@ -18361,7 +18360,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00184','CM047','DO-45892506 ','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="188" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>2896</v>
       </c>
@@ -18403,7 +18402,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00185','CM047','DO-45892506 ','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="189" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>2897</v>
       </c>
@@ -18487,7 +18486,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00187','CM047','DO-45892506 ','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="191" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>2899</v>
       </c>
@@ -18529,7 +18528,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00188','CM047','DO-45892506 ','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="192" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>2900</v>
       </c>
@@ -18613,7 +18612,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00190','CM053','DO-40567939','ZOOM','A','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="194" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>2902</v>
       </c>
@@ -18655,7 +18654,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00191','CM053','DO-40567939','ZOOM','B','4','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="195" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>2903</v>
       </c>
@@ -18739,7 +18738,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00193','CM053','DO-40567939','ZOOM','A','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="197" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>2905</v>
       </c>
@@ -18781,7 +18780,7 @@
         <v>INSERT INTO tbl_Clase(codigo,codigoCurso,codigoDocente,enlace,seccion,grado,periodo,numeroSemanas,fechaInicio,fechaFin) values ('CL2020-00194','CM053','DO-40567939','ZOOM','B','5','2021','40','14/02/2021','14/12/2021');</v>
       </c>
     </row>
-    <row r="198" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>2906</v>
       </c>
@@ -18824,19 +18823,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H198" xr:uid="{3159A5A0-87CD-4305-A3F0-23D1B0D7AA17}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B3:H198" xr:uid="{3159A5A0-87CD-4305-A3F0-23D1B0D7AA17}"/>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A8:A12 A15:A20">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>$B$23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18859,11 +18852,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>2636</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -18902,7 +18895,7 @@
   <dimension ref="A4:R455"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E471" sqref="E471"/>
+      <selection activeCell="F488" sqref="F488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42969,7 +42962,7 @@
   <dimension ref="D3:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I29"/>
+      <selection activeCell="D4" sqref="D4:Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>